<commit_message>
Implementação do teste unitário para o model codest
</commit_message>
<xml_diff>
--- a/resources/Template.xlsx
+++ b/resources/Template.xlsx
@@ -148,122 +148,173 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="146">
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>translation</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>ruleswd</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>rulesvb</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>noun</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>preposition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>tkeyword</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ruleskw</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>adjective</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>pronoun</t>
+  </si>
   <si>
     <t>Code Group Question</t>
   </si>
   <si>
-    <t>Código</t>
+    <t>Alguma regra</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Algum valor</t>
+  </si>
+  <si>
+    <t>answer</t>
   </si>
   <si>
     <t>Code Group ANswer</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
     <t>C0</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Valor</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>questionnaire</t>
   </si>
   <si>
     <t>C8</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>translwd</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>C7</t>
   </si>
   <si>
-    <t>Alguma regra</t>
-  </si>
-  <si>
-    <t>Algum valor</t>
-  </si>
-  <si>
-    <t>rule</t>
-  </si>
-  <si>
-    <t>translation</t>
-  </si>
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>ruleswd</t>
-  </si>
-  <si>
-    <t>verb</t>
-  </si>
-  <si>
-    <t>rulesvb</t>
-  </si>
-  <si>
-    <t>noun</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>preposition</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>tkeyword</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>ruleskw</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>adjective</t>
-  </si>
-  <si>
-    <t>pronoun</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>questionnaire</t>
-  </si>
-  <si>
-    <t>translwd</t>
-  </si>
-  <si>
     <t>translvb</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>translkw</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>translnn</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>translpp</t>
   </si>
   <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>translnb</t>
   </si>
   <si>
@@ -303,15 +354,27 @@
     <t>grouppp</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>groupnb</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>groupadj</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>grouppron</t>
   </si>
   <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>groupwd</t>
   </si>
   <si>
@@ -327,6 +390,24 @@
     <t>1C0</t>
   </si>
   <si>
+    <t>code Group Verb</t>
+  </si>
+  <si>
+    <t>Ordenado</t>
+  </si>
+  <si>
+    <t>Permitir Heranca</t>
+  </si>
+  <si>
+    <t>Código Grupo Pai</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
     <t>Tell me a name of {algum group} please</t>
   </si>
   <si>
@@ -351,33 +432,15 @@
     <t>c</t>
   </si>
   <si>
+    <t>Grupo de respostas</t>
+  </si>
+  <si>
     <t>d</t>
   </si>
   <si>
     <t>z</t>
   </si>
   <si>
-    <t>code Group Verb</t>
-  </si>
-  <si>
-    <t>Ordenado</t>
-  </si>
-  <si>
-    <t>Permitir Heranca</t>
-  </si>
-  <si>
-    <t>Código Grupo Pai</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
-    <t>Grupo de respostas</t>
-  </si>
-  <si>
     <t>1C0 D0 90 D1</t>
   </si>
   <si>
@@ -459,9 +522,15 @@
     <t>wrongs words</t>
   </si>
   <si>
+    <t>Código Keyword</t>
+  </si>
+  <si>
     <t>Código TKeyword</t>
   </si>
   <si>
+    <t>E0</t>
+  </si>
+  <si>
     <t>D0</t>
   </si>
   <si>
@@ -477,12 +546,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Código Keyword</t>
-  </si>
-  <si>
-    <t>E0</t>
-  </si>
-  <si>
     <t>F0</t>
   </si>
   <si>
@@ -507,13 +570,13 @@
     <t>Código Word</t>
   </si>
   <si>
+    <t>Código Preposition</t>
+  </si>
+  <si>
     <t>Código Number</t>
   </si>
   <si>
     <t>1A0</t>
-  </si>
-  <si>
-    <t>Código Preposition</t>
   </si>
   <si>
     <t>Código Adjective</t>
@@ -561,10 +624,10 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -705,275 +768,275 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>9.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
-        <v>11.0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
-        <v>12.0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
-        <v>13.0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
-        <v>14.0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>33</v>
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2">
-        <v>16.0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>35</v>
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2">
-        <v>17.0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
-        <v>18.0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2">
-        <v>19.0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>38</v>
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>40</v>
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>42</v>
+      <c r="A26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>44</v>
+      <c r="A27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>46</v>
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>48</v>
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>50</v>
+      <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>51</v>
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2">
-        <v>21.0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>52</v>
+      <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2">
-        <v>22.0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>53</v>
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2">
-        <v>23.0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>54</v>
+      <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35">
@@ -3886,24 +3949,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>85</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>60.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>10.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>50.0</v>
       </c>
     </row>
@@ -3920,40 +3983,40 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>70.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>86</v>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>71.0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>87</v>
+      <c r="B3" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>72.0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>88</v>
+      <c r="B4" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3968,24 +4031,24 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>80.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>10.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>70.0</v>
       </c>
     </row>
@@ -4002,19 +4065,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>90.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
+      <c r="B2" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4030,24 +4093,24 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
+      <c r="A1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2">
         <v>10.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>90.0</v>
       </c>
     </row>
@@ -4064,19 +4127,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>96</v>
+      <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -4092,37 +4155,37 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
+      <c r="A3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>102</v>
+      <c r="A4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4138,41 +4201,41 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>103</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>99</v>
+      <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>108</v>
+      <c r="A4" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4188,25 +4251,25 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="2">
         <v>10.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>104</v>
+      <c r="C2" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4222,19 +4285,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>112</v>
+      <c r="A2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4254,27 +4317,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4290,19 +4353,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>100.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -4318,19 +4381,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>110.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>114</v>
+      <c r="B2" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4346,19 +4409,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>120.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>115</v>
+      <c r="B2" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4377,24 +4440,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>117</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>140.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>130.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>120.0</v>
       </c>
     </row>
@@ -4414,24 +4477,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>118</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>150.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>50.0</v>
       </c>
     </row>
@@ -4451,25 +4514,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>170.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>104</v>
+      <c r="C2" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4488,24 +4551,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>180.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>90.0</v>
       </c>
     </row>
@@ -4526,25 +4589,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>121</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>190.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>95</v>
+      <c r="C2" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4563,25 +4626,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>111</v>
+      <c r="C2" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4600,24 +4663,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>100.0</v>
       </c>
     </row>
@@ -4638,26 +4701,26 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>10.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4676,24 +4739,24 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>110.0</v>
       </c>
     </row>
@@ -4714,105 +4777,105 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2">
         <v>70.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.0</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="2">
         <v>71.0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>1.0</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="2">
         <v>72.0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>2.0</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>17</v>
+      <c r="A10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="E11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>62</v>
+      <c r="E11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>63</v>
+      <c r="A12" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>64</v>
+      <c r="A15" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>62</v>
+      <c r="A16" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>65</v>
+      <c r="A17" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>66</v>
+      <c r="A18" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>67</v>
+      <c r="A19" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>68</v>
+      <c r="A20" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -4835,47 +4898,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>74</v>
+      <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="1" t="b">
+      <c r="A2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="b">
+      <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.0</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="2">
         <v>5.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="1"/>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -4891,19 +4954,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>130.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>76</v>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4920,43 +4983,43 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>30.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>77</v>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>31.0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>78</v>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>32.0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>79</v>
+      <c r="B4" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>33.0</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>80</v>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4975,32 +5038,32 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>160.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>30.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>70.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>161.0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>32.0</v>
       </c>
     </row>
@@ -5017,19 +5080,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>50.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>83</v>
+      <c r="B2" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>